<commit_message>
Following load and reorganized
</commit_message>
<xml_diff>
--- a/examples/structural/curved_data.xlsx
+++ b/examples/structural/curved_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6975" windowHeight="6000" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6975" windowHeight="6000"/>
   </bookViews>
   <sheets>
     <sheet name="Ghuku (2016)" sheetId="2" r:id="rId1"/>
@@ -18,9 +18,6 @@
     <sheet name="Ghuku (2016) - Fig 10" sheetId="1" r:id="rId4"/>
     <sheet name="Chen (2010)" sheetId="4" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-  </externalReferences>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
@@ -554,10 +551,10 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3174,6 +3171,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3568,6 +3566,7 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -6231,19 +6230,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="xyToExcel"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6509,7 +6495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
@@ -6974,30 +6960,30 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4" t="s">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4" t="s">
+      <c r="F14" s="5"/>
+      <c r="G14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4" t="s">
+      <c r="H14" s="5"/>
+      <c r="I14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4" t="s">
+      <c r="J14" s="5"/>
+      <c r="K14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L14" s="4"/>
+      <c r="L14" s="5"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -7894,51 +7880,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>6.453392813504836E-34</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>1.3416515793369717E-33</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>6.453392813504836E-34</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>5.0006095319986343E-2</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>9.7290222765877843E-4</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>6.0940569710510317E-6</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>-2.7709774440154433E-4</v>
       </c>
       <c r="G3" t="s">
@@ -7946,16 +7932,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>0.10002018511295319</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>1.3913749717175961E-3</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>2.018236045842059E-5</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>-1.1086249724030495E-3</v>
       </c>
       <c r="G4">
@@ -7966,16 +7952,16 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>0.15010295808315277</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>3.7872146349400282E-3</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>1.0294888488715515E-4</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>-2.4627854581922293E-3</v>
       </c>
       <c r="G5">
@@ -7986,16 +7972,16 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>0.2002079039812088</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>5.6861052289605141E-3</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>2.0790637063328177E-4</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>-4.313894547522068E-3</v>
       </c>
       <c r="G6">
@@ -8006,16 +7992,16 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>0.2504427433013916</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>9.6172690391540527E-3</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>4.4275730033405125E-4</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>-6.6327308304607868E-3</v>
       </c>
       <c r="G7">
@@ -8026,16 +8012,16 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>0.30071151256561279</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>1.3108834624290466E-2</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>7.1150175062939525E-4</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>-9.3911662697792053E-3</v>
       </c>
       <c r="G8">
@@ -8046,51 +8032,51 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>0.35116297006607056</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>1.8687227740883827E-2</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>1.1629753280431032E-3</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>-1.2562771327793598E-2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>0.40165713429450989</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>2.3883387446403503E-2</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>1.6571145970374346E-3</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>-1.6116611659526825E-2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>0.4523780345916748</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>3.1220881268382072E-2</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>2.3780330084264278E-3</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>-2.0029118284583092E-2</v>
       </c>
       <c r="G11">
         <f>-G4</f>
         <v>0</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <f>-H4</f>
         <v>0</v>
       </c>
@@ -8099,23 +8085,23 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>0.50314706563949585</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>3.8233637809753418E-2</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>3.1470682006329298E-3</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>-2.4266362190246582E-2</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <f t="shared" ref="G12:H15" si="0">-G5</f>
         <v>2.5</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="4">
         <f t="shared" si="0"/>
         <v>2.170681E-2</v>
       </c>
@@ -8124,23 +8110,23 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>0.55417782068252563</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>4.7442477196455002E-2</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>4.1777808219194412E-3</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>-2.8807524591684341E-2</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="4">
         <f t="shared" si="0"/>
         <v>4.7649450000000003E-2</v>
       </c>
@@ -8149,23 +8135,23 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>0.60525840520858765</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>5.6384321302175522E-2</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>5.2583832293748856E-3</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>-3.3615682274103165E-2</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="4">
         <f t="shared" si="0"/>
         <v>7.6165479999999994E-2</v>
       </c>
@@ -8174,23 +8160,23 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>0.65662604570388794</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>6.7577548325061798E-2</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>6.6260644234716892E-3</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>-3.8672454655170441E-2</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="4">
         <f t="shared" si="0"/>
         <v>0.10340379</v>
       </c>
@@ -8199,100 +8185,100 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>0.70804136991500854</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>7.8561894595623016E-2</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>8.0413883551955223E-3</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>-4.3938111513853073E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="4">
         <v>0.75975936651229858</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>9.1853752732276917E-2</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>9.7593488171696663E-3</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>-4.9396246671676636E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>0.81151837110519409</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>0.10499536991119385</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>1.1518340557813644E-2</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>-5.5004626512527466E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="A19" s="4">
         <v>0.86358535289764404</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>0.12050178647041321</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>1.3585310429334641E-2</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>-6.074821949005127E-2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="A20" s="4">
         <v>0.91568195819854736</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>0.13591727614402771</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>1.5681957826018333E-2</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <v>-6.6582731902599335E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="A21" s="4">
         <v>0.96808129549026489</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4">
         <v>0.15375615656375885</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <v>1.8081283196806908E-2</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
         <v>-7.249382883310318E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="A22" s="4">
         <v>1.0204937458038299</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>0.17156435549259186</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>2.04937644302845E-2</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <v>-7.8435644507408142E-2</v>
       </c>
     </row>

</xml_diff>